<commit_message>
Added functionality for working with files.
</commit_message>
<xml_diff>
--- a/doc/Plans/План.xlsx
+++ b/doc/Plans/План.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11955"/>
@@ -494,7 +494,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -530,7 +530,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="3">
-        <v>41750</v>
+        <v>41821</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
@@ -550,7 +550,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="3">
-        <v>41764</v>
+        <v>41835</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
@@ -565,12 +565,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="93.75">
+    <row r="4" spans="1:6" ht="75">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="3">
-        <v>41805</v>
+        <v>41883</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>8</v>
@@ -585,12 +585,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="56.25">
+    <row r="5" spans="1:6" ht="37.5">
       <c r="A5" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="3">
-        <v>41852</v>
+        <v>41927</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>30</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="3">
-        <v>41913</v>
+        <v>41958</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="37.5">
@@ -625,7 +625,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="168.75">
+    <row r="10" spans="1:6" ht="131.25">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
@@ -637,7 +637,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="37.5">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -651,7 +651,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="56.25">
+    <row r="13" spans="1:6" ht="37.5">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -675,7 +675,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="37.5">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>

</xml_diff>